<commit_message>
proceeded with paper code
</commit_message>
<xml_diff>
--- a/04_Writing/02_Tables/tab_cleantech_market.xlsx
+++ b/04_Writing/02_Tables/tab_cleantech_market.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Meine Bibliotheken\Research\01_Promotion\05_Ideas\09_Cleantech\cleantech\04_Writing\02_Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dokumente\Jobs\ZEW\Research\01_Promotion\05_Ideas\09_Cleantech\cleantech\04_Writing\02_Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437EDB04-85C0-4731-BC3F-A9C25DDA2939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,77 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
-  <si>
-    <t>Clean technology market</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>CPC group</t>
   </si>
   <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
     <t>&amp;</t>
   </si>
   <si>
     <t>\\</t>
   </si>
   <si>
-    <t>Adaption</t>
-  </si>
-  <si>
-    <t>Battery</t>
-  </si>
-  <si>
-    <t>Biofuels</t>
-  </si>
-  <si>
-    <t>Adaption to climate change</t>
-  </si>
-  <si>
-    <t>Battery storage and fuel cells</t>
-  </si>
-  <si>
-    <t>Carbon capture, storage and sequestration</t>
-  </si>
-  <si>
-    <t>CCS</t>
-  </si>
-  <si>
-    <t>Electric vehicles and low carbon mobility solutions</t>
-  </si>
-  <si>
-    <t>Mobility</t>
-  </si>
-  <si>
-    <t>Energy efficiency</t>
-  </si>
-  <si>
-    <t>E-efficiency</t>
-  </si>
-  <si>
-    <t>Low carbon materials and manufacturing</t>
-  </si>
-  <si>
-    <t>Materials</t>
-  </si>
-  <si>
-    <t>Renewable energy generation</t>
-  </si>
-  <si>
-    <t>Generation</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Environmental data, software, finance, consultancy</t>
-  </si>
-  <si>
-    <t>ICT</t>
-  </si>
-  <si>
     <t>Y02B 90/10, Y02E 60/30, Y02E 60/32, Y02E 60/34, Y02E 60/36, Y02E 60/50, Y02E 60/30, Y02P 90/40, Y02P 90/45, Y02P 90/50, Y02T 90/40</t>
   </si>
   <si>
@@ -107,15 +48,6 @@
     <t>Y02B 20-50, Y02B 70, Y02B 90 (Y02B 90/10), Y02D 10, Y02D 30, Y02D 70, Y02E 20, Y02E 40, Y02P 80</t>
   </si>
   <si>
-    <t>Y02P 90 (except Y02P 90/40, Y02P 90/45, Y02P 90/50, Y02P 90/70)</t>
-  </si>
-  <si>
-    <t>Grid and power conversion</t>
-  </si>
-  <si>
-    <t>Grid</t>
-  </si>
-  <si>
     <t>Y02T 10 (except Y02T 10/30, Y02T 10/70), Y02T 30, Y02T 50, Y02T 70, Y02T 90 (except Y02T 90/40)</t>
   </si>
   <si>
@@ -134,13 +66,76 @@
     <t>Y02A 10, Y02A 30-60, Y02A 90, Y02B 80</t>
   </si>
   <si>
-    <t>Water and wastewater treatment</t>
+    <t>Battery storage and fuel cells (Battery)</t>
+  </si>
+  <si>
+    <t>Carbon capture, storage and sequestration (CCS)</t>
+  </si>
+  <si>
+    <t>Electric vehicles and low carbon mobility solutions (Mobility)</t>
+  </si>
+  <si>
+    <t>Energy efficiency (E-efficiency)</t>
+  </si>
+  <si>
+    <t>Grid and power conversion (Grid)</t>
+  </si>
+  <si>
+    <t>Low carbon materials and manufacturing (Materials)</t>
+  </si>
+  <si>
+    <t>Renewable energy generation (Generation)</t>
+  </si>
+  <si>
+    <t>Water and wastewater treatment (Water)</t>
+  </si>
+  <si>
+    <t>Technologies for the adaption to climate change (Adaption)</t>
+  </si>
+  <si>
+    <t>Biofuel technologies (Biofuels)</t>
+  </si>
+  <si>
+    <t>Clean technology field</t>
+  </si>
+  <si>
+    <t>Technology example</t>
+  </si>
+  <si>
+    <t>Enhanced coal bed methane recovery</t>
+  </si>
+  <si>
+    <t>Genetically modified plants resistant to drought</t>
+  </si>
+  <si>
+    <t>Generation of geothermal energy</t>
+  </si>
+  <si>
+    <t>Fuel cell technologies in production processes</t>
+  </si>
+  <si>
+    <t>Algae biomass</t>
+  </si>
+  <si>
+    <t>Ultracapacitors for efficient electric vehicle charging</t>
+  </si>
+  <si>
+    <t>Insulation technologies inhibiting radiant heat transfer</t>
+  </si>
+  <si>
+    <t>Smart grids</t>
+  </si>
+  <si>
+    <t>Technologies for the production of fertilisers from the organic fraction of waste or refuse</t>
+  </si>
+  <si>
+    <t>Technologies to replace cement by fly ash in concrete production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,8 +179,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,254 +457,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F13" s="1"/>
@@ -729,14 +707,11 @@
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
-    <hyperlink ref="F2:F19" r:id="rId2" display="\\"/>
-    <hyperlink ref="F9" r:id="rId3"/>
+    <hyperlink ref="F1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2:F18" r:id="rId2" display="\\" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>